<commit_message>
AIP-400 AIP-443 Removed TestData File
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_95_BTC106.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_95_BTC106.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D6F3F7-AAD6-4AFE-8BA0-7E728C051E79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A40C35-B993-4AE3-AC70-967576716251}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="163">
   <si>
     <t>DeviceType</t>
   </si>
@@ -58,12 +58,6 @@
     <t>Mountain Standard Time</t>
   </si>
   <si>
-    <t>Mexico Standard Time 2</t>
-  </si>
-  <si>
-    <t>U.S. Mountain Standard Time</t>
-  </si>
-  <si>
     <t>(GMT-07:00) Arizona</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>(GMT-06:00) Saskatchewan</t>
   </si>
   <si>
-    <t>Mexico Standard Time</t>
-  </si>
-  <si>
     <t>(GMT-06:00) Guadalajara, Mexico City, Monterrey</t>
   </si>
   <si>
@@ -91,15 +82,9 @@
     <t>Eastern Standard Time</t>
   </si>
   <si>
-    <t>U.S. Eastern Standard Time</t>
-  </si>
-  <si>
     <t>(GMT-05:00) Indiana (East)</t>
   </si>
   <si>
-    <t>S.A. Pacific Standard Time</t>
-  </si>
-  <si>
     <t>(GMT-05:00) Bogota, Lima, Quito</t>
   </si>
   <si>
@@ -109,18 +94,9 @@
     <t>(GMT-04:00) Atlantic Time (Canada)</t>
   </si>
   <si>
-    <t>S.A. Western Standard Time</t>
-  </si>
-  <si>
-    <t>Pacific S.A. Standard Time</t>
-  </si>
-  <si>
     <t>(GMT-04:00) Santiago</t>
   </si>
   <si>
-    <t>Newfoundland and Labrador Standard Time</t>
-  </si>
-  <si>
     <t>E. South America Standard Time</t>
   </si>
   <si>
@@ -509,6 +485,33 @@
   </si>
   <si>
     <t>409026540</t>
+  </si>
+  <si>
+    <t>Dateline Standard Time</t>
+  </si>
+  <si>
+    <t>Mountain Standard Time (Mexico)</t>
+  </si>
+  <si>
+    <t>US Mountain Standard Time</t>
+  </si>
+  <si>
+    <t>Central Standard Time (Mexico)</t>
+  </si>
+  <si>
+    <t>US Eastern Standard Time</t>
+  </si>
+  <si>
+    <t>SA Pacific Standard Time</t>
+  </si>
+  <si>
+    <t>SA Western Standard Time</t>
+  </si>
+  <si>
+    <t>Pacific SA Standard Time</t>
+  </si>
+  <si>
+    <t>Newfoundland Standard Time</t>
   </si>
 </sst>
 </file>
@@ -874,7 +877,7 @@
   <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,10 +892,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -901,39 +904,39 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" t="s">
         <v>154</v>
-      </c>
-      <c r="D2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G2" t="s">
-        <v>81</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
@@ -941,22 +944,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
@@ -967,22 +970,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -993,22 +996,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -1019,1848 +1022,1844 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" t="s">
-        <v>159</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>155</v>
       </c>
       <c r="H8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E9" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C10" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D11" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E12" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>157</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D13" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E13" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D14" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E14" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C15" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E15" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="H15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" t="s">
         <v>159</v>
       </c>
-      <c r="B16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C16" t="s">
-        <v>154</v>
-      </c>
-      <c r="D16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" t="s">
-        <v>160</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G16" t="s">
-        <v>24</v>
-      </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E17" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D18" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E18" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" t="s">
         <v>160</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G18" t="s">
-        <v>28</v>
-      </c>
       <c r="H18" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E19" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G19" t="s">
         <v>161</v>
       </c>
-      <c r="G19" t="s">
-        <v>29</v>
-      </c>
       <c r="H19" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C20" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E20" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G20" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="H20" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E21" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G21" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H21" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E22" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G22" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H22" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C23" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E23" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G23" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H23" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C24" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E24" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G24" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H24" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B25" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C25" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D25" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E25" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G25" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H25" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B26" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C26" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D26" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E26" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G26" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H26" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C27" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D27" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E27" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G27" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H27" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C28" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D28" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E28" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H28" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C29" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E29" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G29" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H29" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B30" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C30" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D30" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E30" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G30" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H30" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C31" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G31" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H31" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D32" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E32" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G32" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H32" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B33" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D33" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E33" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G33" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H33" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C34" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D34" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E34" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G34" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H34" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B35" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D35" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E35" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G35" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H35" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B36" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C36" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E36" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G36" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H36" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B37" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C37" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D37" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E37" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G37" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H37" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C38" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E38" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G38" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H38" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B39" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C39" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D39" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E39" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G39" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H39" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E40" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G40" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H40" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C41" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E41" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G41" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C42" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E42" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G42" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H42" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B43" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D43" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E43" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G43" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H43" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C44" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D44" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E44" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G44" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H44" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C45" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D45" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E45" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G45" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H45" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C46" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D46" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E46" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G46" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H46" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D47" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E47" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G47" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="H47" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C48" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D48" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E48" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G48" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H48" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C49" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D49" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E49" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G49" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H49" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B50" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C50" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E50" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G50" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H50" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B51" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C51" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D51" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E51" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G51" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H51" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C52" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D52" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E52" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G52" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H52" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B53" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D53" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E53" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G53" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H53" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B54" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C54" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D54" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E54" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G54" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="H54" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B55" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C55" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D55" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E55" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G55" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H55" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B56" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C56" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D56" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E56" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G56" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="H56" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B57" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C57" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D57" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E57" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G57" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H57" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B58" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D58" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E58" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G58" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="H58" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D59" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E59" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G59" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H59" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B60" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C60" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D60" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E60" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G60" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H60" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B61" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C61" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D61" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E61" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G61" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H61" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B62" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C62" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D62" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E62" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G62" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H62" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C63" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D63" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E63" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G63" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="H63" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B64" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C64" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D64" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E64" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G64" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H64" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B65" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C65" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D65" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E65" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G65" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H65" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B66" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C66" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D66" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E66" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G66" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="H66" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B67" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C67" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D67" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E67" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G67" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H67" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B68" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D68" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E68" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G68" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="H68" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B69" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C69" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D69" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E69" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G69" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H69" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B70" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C70" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D70" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E70" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G70" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="H70" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B71" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C71" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D71" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E71" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G71" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H71" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B72" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C72" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D72" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E72" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G72" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H72" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C73" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D73" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E73" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G73" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H73" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B74" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C74" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D74" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E74" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G74" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="H74" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C75" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D75" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E75" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G75" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="H75" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C76" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D76" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E76" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G76" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="H76" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "AIP-400 AIP-443 Removed TestData File"
This reverts commit 73d3c63c003632d20007a9ce5b0448c85efa5238.
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_95_BTC106.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_95_BTC106.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A40C35-B993-4AE3-AC70-967576716251}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D6F3F7-AAD6-4AFE-8BA0-7E728C051E79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="162">
   <si>
     <t>DeviceType</t>
   </si>
@@ -58,6 +58,12 @@
     <t>Mountain Standard Time</t>
   </si>
   <si>
+    <t>Mexico Standard Time 2</t>
+  </si>
+  <si>
+    <t>U.S. Mountain Standard Time</t>
+  </si>
+  <si>
     <t>(GMT-07:00) Arizona</t>
   </si>
   <si>
@@ -70,6 +76,9 @@
     <t>(GMT-06:00) Saskatchewan</t>
   </si>
   <si>
+    <t>Mexico Standard Time</t>
+  </si>
+  <si>
     <t>(GMT-06:00) Guadalajara, Mexico City, Monterrey</t>
   </si>
   <si>
@@ -82,9 +91,15 @@
     <t>Eastern Standard Time</t>
   </si>
   <si>
+    <t>U.S. Eastern Standard Time</t>
+  </si>
+  <si>
     <t>(GMT-05:00) Indiana (East)</t>
   </si>
   <si>
+    <t>S.A. Pacific Standard Time</t>
+  </si>
+  <si>
     <t>(GMT-05:00) Bogota, Lima, Quito</t>
   </si>
   <si>
@@ -94,9 +109,18 @@
     <t>(GMT-04:00) Atlantic Time (Canada)</t>
   </si>
   <si>
+    <t>S.A. Western Standard Time</t>
+  </si>
+  <si>
+    <t>Pacific S.A. Standard Time</t>
+  </si>
+  <si>
     <t>(GMT-04:00) Santiago</t>
   </si>
   <si>
+    <t>Newfoundland and Labrador Standard Time</t>
+  </si>
+  <si>
     <t>E. South America Standard Time</t>
   </si>
   <si>
@@ -485,33 +509,6 @@
   </si>
   <si>
     <t>409026540</t>
-  </si>
-  <si>
-    <t>Dateline Standard Time</t>
-  </si>
-  <si>
-    <t>Mountain Standard Time (Mexico)</t>
-  </si>
-  <si>
-    <t>US Mountain Standard Time</t>
-  </si>
-  <si>
-    <t>Central Standard Time (Mexico)</t>
-  </si>
-  <si>
-    <t>US Eastern Standard Time</t>
-  </si>
-  <si>
-    <t>SA Pacific Standard Time</t>
-  </si>
-  <si>
-    <t>SA Western Standard Time</t>
-  </si>
-  <si>
-    <t>Pacific SA Standard Time</t>
-  </si>
-  <si>
-    <t>Newfoundland Standard Time</t>
   </si>
 </sst>
 </file>
@@ -877,7 +874,7 @@
   <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,10 +889,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -904,39 +901,39 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G2" t="s">
-        <v>154</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
@@ -944,22 +941,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E3" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
@@ -970,22 +967,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -996,22 +993,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
@@ -1022,1844 +1019,1848 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
+      <c r="A7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" t="s">
+        <v>159</v>
+      </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E7" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G9" t="s">
-        <v>156</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E10" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E11" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D12" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G12" t="s">
-        <v>157</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E14" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G15" t="s">
-        <v>158</v>
+        <v>22</v>
       </c>
       <c r="H15" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E16" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G16" t="s">
-        <v>159</v>
+        <v>24</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="H17" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G18" t="s">
-        <v>160</v>
+        <v>28</v>
       </c>
       <c r="H18" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C19" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E19" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G19" t="s">
-        <v>161</v>
+        <v>29</v>
       </c>
       <c r="H19" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G20" t="s">
-        <v>162</v>
+        <v>31</v>
       </c>
       <c r="H20" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E21" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G21" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="H21" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" t="s">
         <v>145</v>
       </c>
-      <c r="E22" t="s">
-        <v>152</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G22" t="s">
-        <v>137</v>
-      </c>
       <c r="H22" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C23" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D23" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E23" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="H23" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C24" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E24" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G24" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H24" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E25" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G25" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H25" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G26" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H26" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D27" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E27" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G27" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H27" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C28" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D28" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E28" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G28" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H28" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C29" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D29" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E29" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G29" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H29" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B30" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D30" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E30" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G30" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="H30" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C31" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D31" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E31" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G31" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H31" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C32" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D32" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E32" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G32" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H32" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D33" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E33" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G33" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H33" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D34" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E34" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G34" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H34" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C35" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D35" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E35" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G35" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H35" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C36" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G36" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H36" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C37" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D37" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E37" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G37" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="H37" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C38" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G38" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H38" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B39" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C39" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D39" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E39" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G39" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="H39" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D40" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E40" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G40" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H40" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B41" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D41" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E41" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G41" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="H41" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B42" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C42" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E42" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G42" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H42" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C43" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E43" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G43" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="H43" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D44" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E44" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G44" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="H44" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B45" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C45" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D45" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E45" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G45" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="H45" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B46" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C46" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E46" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G46" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="H46" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B47" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C47" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D47" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E47" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G47" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="H47" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B48" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C48" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D48" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E48" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G48" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="H48" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B49" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D49" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E49" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G49" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="H49" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B50" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D50" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E50" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G50" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="H50" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D51" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E51" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G51" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="H51" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C52" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D52" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E52" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G52" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H52" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B53" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E53" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G53" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H53" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B54" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C54" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D54" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E54" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G54" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="H54" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D55" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E55" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G55" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H55" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C56" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D56" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E56" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G56" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="H56" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B57" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D57" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E57" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G57" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="H57" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B58" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C58" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D58" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E58" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G58" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="H58" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B59" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D59" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E59" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G59" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="H59" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B60" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D60" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E60" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G60" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="H60" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B61" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C61" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D61" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E61" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G61" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="H61" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B62" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C62" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D62" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E62" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G62" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H62" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B63" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C63" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D63" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E63" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G63" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="H63" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B64" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D64" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E64" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G64" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="H64" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B65" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C65" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D65" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E65" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G65" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="H65" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B66" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C66" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D66" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E66" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G66" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="H66" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B67" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D67" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E67" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G67" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H67" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B68" t="s">
+        <v>159</v>
+      </c>
+      <c r="C68" t="s">
+        <v>154</v>
+      </c>
+      <c r="D68" t="s">
+        <v>153</v>
+      </c>
+      <c r="E68" t="s">
+        <v>160</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G68" t="s">
         <v>151</v>
       </c>
-      <c r="B68" t="s">
-        <v>151</v>
-      </c>
-      <c r="C68" t="s">
-        <v>146</v>
-      </c>
-      <c r="D68" t="s">
-        <v>145</v>
-      </c>
-      <c r="E68" t="s">
-        <v>152</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G68" t="s">
-        <v>143</v>
-      </c>
       <c r="H68" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B69" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C69" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D69" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E69" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G69" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="H69" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B70" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C70" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D70" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E70" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G70" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="H70" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B71" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C71" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D71" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E71" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G71" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="H71" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B72" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C72" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D72" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E72" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G72" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="H72" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B73" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C73" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D73" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E73" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G73" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="H73" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B74" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D74" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E74" t="s">
+        <v>160</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G74" t="s">
         <v>152</v>
       </c>
-      <c r="F74" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>144</v>
-      </c>
-      <c r="H74" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B75" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C75" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D75" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E75" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G75" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="H75" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B76" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C76" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D76" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E76" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G76" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="H76" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AIP-392 AIP-568 Corrected Test Data for GMT-12
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_95_BTC106.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_95_BTC106.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D6F3F7-AAD6-4AFE-8BA0-7E728C051E79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D95368-12FD-41EF-86D3-760DE2A49ED2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$75</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="163">
   <si>
     <t>DeviceType</t>
   </si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t>409026540</t>
+  </si>
+  <si>
+    <t>Dateline Standard Time</t>
   </si>
 </sst>
 </file>
@@ -873,8 +876,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +936,7 @@
         <v>161</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
@@ -2181,10 +2184,10 @@
         <v>161</v>
       </c>
       <c r="G50" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H50" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2207,10 +2210,10 @@
         <v>161</v>
       </c>
       <c r="G51" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H51" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2233,10 +2236,10 @@
         <v>161</v>
       </c>
       <c r="G52" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2259,10 +2262,10 @@
         <v>161</v>
       </c>
       <c r="G53" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H53" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2285,10 +2288,10 @@
         <v>161</v>
       </c>
       <c r="G54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H54" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2311,10 +2314,10 @@
         <v>161</v>
       </c>
       <c r="G55" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="H55" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2337,10 +2340,10 @@
         <v>161</v>
       </c>
       <c r="G56" t="s">
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="H56" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2363,10 +2366,10 @@
         <v>161</v>
       </c>
       <c r="G57" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H57" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2389,10 +2392,10 @@
         <v>161</v>
       </c>
       <c r="G58" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H58" t="s">
-        <v>141</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2415,10 +2418,10 @@
         <v>161</v>
       </c>
       <c r="G59" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H59" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2441,10 +2444,10 @@
         <v>161</v>
       </c>
       <c r="G60" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H60" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2467,10 +2470,10 @@
         <v>161</v>
       </c>
       <c r="G61" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H61" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2493,10 +2496,10 @@
         <v>161</v>
       </c>
       <c r="G62" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H62" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2519,10 +2522,10 @@
         <v>161</v>
       </c>
       <c r="G63" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H63" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2545,10 +2548,10 @@
         <v>161</v>
       </c>
       <c r="G64" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H64" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2571,10 +2574,10 @@
         <v>161</v>
       </c>
       <c r="G65" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="H65" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2597,10 +2600,10 @@
         <v>161</v>
       </c>
       <c r="G66" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
       <c r="H66" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2623,10 +2626,10 @@
         <v>161</v>
       </c>
       <c r="G67" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
       <c r="H67" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2649,10 +2652,10 @@
         <v>161</v>
       </c>
       <c r="G68" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="H68" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2675,10 +2678,10 @@
         <v>161</v>
       </c>
       <c r="G69" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H69" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2701,10 +2704,10 @@
         <v>161</v>
       </c>
       <c r="G70" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H70" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2727,10 +2730,10 @@
         <v>161</v>
       </c>
       <c r="G71" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H71" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2753,10 +2756,10 @@
         <v>161</v>
       </c>
       <c r="G72" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H72" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2779,10 +2782,10 @@
         <v>161</v>
       </c>
       <c r="G73" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="H73" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2805,10 +2808,10 @@
         <v>161</v>
       </c>
       <c r="G74" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="H74" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -2831,10 +2834,10 @@
         <v>161</v>
       </c>
       <c r="G75" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H75" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2857,10 +2860,10 @@
         <v>161</v>
       </c>
       <c r="G76" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="H76" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>